<commit_message>
various additions, clean up of older models
</commit_message>
<xml_diff>
--- a/CYTK.xlsx
+++ b/CYTK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1506BB0F-87BF-4A5E-9721-83DB7A4AAFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EF44ED-F350-4576-AC80-ADA15133114C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22590" yWindow="735" windowWidth="22335" windowHeight="19365" xr2:uid="{A49A7A12-B745-4EC9-B913-D708EFED4797}"/>
+    <workbookView xWindow="-31170" yWindow="1860" windowWidth="19845" windowHeight="16215" activeTab="2" xr2:uid="{A49A7A12-B745-4EC9-B913-D708EFED4797}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -290,7 +290,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -301,7 +300,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,33 +639,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42353201-ED6E-407F-99F1-919EDB88A99D}">
   <dimension ref="B2:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
       <c r="J2" t="s">
         <v>0</v>
       </c>
@@ -679,14 +678,10 @@
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="5"/>
       <c r="J3" t="s">
         <v>1</v>
       </c>
@@ -701,16 +696,13 @@
       <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
       <c r="J4" t="s">
         <v>2</v>
       </c>
@@ -720,19 +712,16 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="5"/>
       <c r="J5" t="s">
         <v>3</v>
       </c>
@@ -748,14 +737,10 @@
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="5"/>
       <c r="J6" t="s">
         <v>4</v>
       </c>
@@ -772,13 +757,10 @@
       <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
       <c r="J7" t="s">
         <v>5</v>
       </c>
@@ -789,21 +771,11 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
       <c r="J9" t="s">
         <v>7</v>
       </c>
@@ -813,12 +785,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
       <c r="J10" t="s">
         <v>8</v>
       </c>
@@ -828,21 +795,16 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
       <c r="J12" t="s">
         <v>9</v>
       </c>
@@ -871,7 +833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820767BF-BF34-44B5-A34D-0C11A3B98053}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -880,7 +844,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -911,7 +875,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -921,22 +885,22 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>